<commit_message>
upload of rainfall and yield data
</commit_message>
<xml_diff>
--- a/rice_yield_1981_2016.xlsx
+++ b/rice_yield_1981_2016.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak97126\Documents\GitHub_com\ubu_data_analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Harvested area</t>
   </si>
   <si>
-    <t>(Rai)</t>
-  </si>
-  <si>
     <t>Yield</t>
-  </si>
-  <si>
-    <t>(tons)</t>
   </si>
   <si>
     <t>Yield per Rai (kg)</t>
@@ -53,11 +52,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="General_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="General_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -124,7 +123,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -169,90 +168,50 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -266,6 +225,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -591,782 +558,763 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="17">
-      <c r="A2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>7</v>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="17">
-      <c r="A3" s="17"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A4" s="10">
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2524</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B3" s="7">
         <v>1981</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C3" s="8">
         <v>3569843</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D3" s="8">
         <v>3327265</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E3" s="8">
         <v>542679</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F3" s="8">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A5" s="10">
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>2525</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B4" s="7">
         <v>1982</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C4" s="8">
         <v>3393766</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D4" s="8">
         <v>3083817</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E4" s="8">
         <v>485860</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F4" s="8">
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A6" s="10">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>2526</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B5" s="7">
         <v>1983</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C5" s="8">
         <v>3352107</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D5" s="8">
         <v>3048922</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E5" s="8">
         <v>586619</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F5" s="8">
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A7" s="10">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>2527</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B6" s="7">
         <v>1984</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C6" s="8">
         <v>3501520</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D6" s="8">
         <v>3420872</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E6" s="8">
         <v>665289</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F6" s="8">
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A8" s="10">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>2528</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B7" s="7">
         <v>1985</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C7" s="8">
         <v>3704958</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D7" s="8">
         <v>2588008</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E7" s="8">
         <v>733582</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F7" s="8">
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A9" s="10">
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>2529</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B8" s="7">
         <v>1986</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C8" s="8">
         <v>3645875</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D8" s="8">
         <v>3606588</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E8" s="8">
         <v>700008</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F8" s="8">
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A10" s="10">
+    <row r="9" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>2530</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B9" s="7">
         <v>1987</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C9" s="8">
         <v>3746372</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D9" s="8">
         <v>3740787</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E9" s="8">
         <v>897789</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F9" s="8">
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A11" s="10">
+    <row r="10" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>2531</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B10" s="7">
         <v>1988</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C10" s="8">
         <v>3729293</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D10" s="8">
         <v>3600508</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E10" s="8">
         <v>742129</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F10" s="8">
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A12" s="10">
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>2532</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B11" s="7">
         <v>1989</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C11" s="8">
         <v>3752830</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D11" s="8">
         <v>3734344</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E11" s="8">
         <v>848140</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F11" s="8">
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A13" s="10">
+    <row r="12" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>2533</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B12" s="7">
         <v>1990</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C12" s="10">
         <v>3838720</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D12" s="10">
         <v>3810819</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E12" s="10">
         <v>909777</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F12" s="8">
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A14" s="10">
+    <row r="13" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>2534</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B13" s="7">
         <v>1991</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C13" s="10">
         <v>3593593</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D13" s="10">
         <v>3458047</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E13" s="10">
         <v>804965</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F13" s="8">
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A15" s="10">
+    <row r="14" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>2535</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B14" s="7">
         <v>1992</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C14" s="10">
         <v>3508727</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D14" s="10">
         <v>3441368</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E14" s="10">
         <v>821042</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F14" s="8">
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A16" s="10">
+    <row r="15" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>2536</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B15" s="7">
         <v>1993</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C15" s="10">
         <v>3432199</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D15" s="10">
         <v>3212881</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E15" s="10">
         <v>713897</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F15" s="8">
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A17" s="10">
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>2537</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B16" s="7">
         <v>1994</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C16" s="10">
         <v>2945927</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D16" s="10">
         <v>2858190</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E16" s="10">
         <v>741530</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F16" s="8">
         <v>259</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A18" s="10">
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>2538</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B17" s="7">
         <v>1995</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C17" s="10">
         <v>2946448</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D17" s="10">
         <v>2723991</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E17" s="10">
         <v>748398</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F17" s="8">
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A19" s="10">
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>2539</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B18" s="7">
         <v>1996</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C18" s="10">
         <v>2891807</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D18" s="10">
         <v>2818081</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E18" s="10">
         <v>686035</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F18" s="8">
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A20" s="10">
+    <row r="19" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>2540</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B19" s="7">
         <v>1997</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C19" s="10">
         <v>2979330</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D19" s="10">
         <v>2910286</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E19" s="10">
         <v>746471</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F19" s="8">
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A21" s="10">
+    <row r="20" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>2541</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B20" s="7">
         <v>1998</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C20" s="10">
         <v>3042863</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D20" s="10">
         <v>2999651</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E20" s="10">
         <v>743247</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F20" s="8">
         <v>248</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A22" s="10">
+    <row r="21" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>2542</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B21" s="7">
         <v>1999</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C21" s="10">
         <v>3097624</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D21" s="10">
         <v>3061557</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E21" s="10">
         <v>796490</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F21" s="8">
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A23" s="10">
+    <row r="22" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>2543</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B22" s="7">
         <v>2000</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C22" s="10">
         <v>3160726</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D22" s="10">
         <v>3018089</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E22" s="10">
         <v>857491</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F22" s="8">
         <v>284</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A24" s="10">
+    <row r="23" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
         <v>2544</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B23" s="7">
         <v>2001</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C23" s="8">
         <v>3363915</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D23" s="8">
         <v>3316356</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E23" s="8">
         <v>1034983</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F23" s="8">
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A25" s="10">
+    <row r="24" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>2545</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B24" s="7">
         <v>2002</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C24" s="8">
         <v>3224240</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D24" s="8">
         <v>3042148</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E24" s="8">
         <v>864197</v>
       </c>
-      <c r="F25" s="11">
+      <c r="F24" s="8">
         <v>284</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A26" s="14">
+    <row r="25" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
         <v>2546</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B25" s="7">
         <v>2003</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C25" s="8">
         <v>3180431</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D25" s="8">
         <v>3116822</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E25" s="8">
         <v>865034</v>
       </c>
-      <c r="F26" s="11">
+      <c r="F25" s="8">
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A27" s="14">
+    <row r="26" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>2547</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B26" s="7">
         <v>2004</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C26" s="8">
         <v>3207179</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D26" s="8">
         <v>3095814</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E26" s="8">
         <v>952143</v>
       </c>
-      <c r="F27" s="11">
+      <c r="F26" s="8">
         <v>308</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A28" s="14">
+    <row r="27" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
         <v>2548</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B27" s="7">
         <v>2005</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C27" s="8">
         <v>3207788</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D27" s="8">
         <v>3062557</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E27" s="8">
         <v>970896</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F27" s="8">
         <v>317</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A29" s="14">
+    <row r="28" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>2549</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B28" s="7">
         <v>2006</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C28" s="8">
         <v>3182153</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D28" s="8">
         <v>3044758</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E28" s="8">
         <v>960100</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F28" s="8">
         <v>315</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A30" s="14">
+    <row r="29" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
         <v>2550</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B29" s="7">
         <v>2007</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C29" s="8">
         <v>3201999</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D29" s="8">
         <v>3026142</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E29" s="8">
         <v>981684</v>
       </c>
-      <c r="F30" s="11">
+      <c r="F29" s="8">
         <v>324</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A31" s="14">
+    <row r="30" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>2551</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B30" s="7">
         <v>2008</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C30" s="8">
         <v>3264948</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D30" s="8">
         <v>3080598</v>
       </c>
-      <c r="E31" s="11">
+      <c r="E30" s="8">
         <v>979196</v>
       </c>
-      <c r="F31" s="11">
+      <c r="F30" s="8">
         <v>318</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A32" s="14">
+    <row r="31" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
         <v>2552</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B31" s="7">
         <v>2009</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C31" s="8">
         <v>3526280</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D31" s="8">
         <v>3312990</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E31" s="8">
         <v>1079125</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F31" s="8">
         <v>326</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A33" s="14">
+    <row r="32" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>2553</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B32" s="7">
         <v>2010</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C32" s="8">
         <v>4195067</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D32" s="8">
         <v>3913827</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E32" s="8">
         <v>1233350</v>
       </c>
-      <c r="F33" s="11">
+      <c r="F32" s="8">
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A34" s="14">
+    <row r="33" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>2554</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B33" s="7">
         <v>2011</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C33" s="8">
         <v>4273111</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D33" s="8">
         <v>4047374</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E33" s="8">
         <v>1396344</v>
       </c>
-      <c r="F34" s="11">
+      <c r="F33" s="8">
         <v>345</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A35" s="14">
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>2555</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B34" s="7">
         <v>2012</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C34" s="8">
         <v>4314831</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D34" s="8">
         <v>4163693</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E34" s="8">
         <v>1432101</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F34" s="8">
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A36" s="14">
+    <row r="35" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
         <v>2556</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B35" s="7">
         <v>2013</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C35" s="8">
         <v>3891535</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D35" s="8">
         <v>3680200</v>
       </c>
-      <c r="E36" s="11">
+      <c r="E35" s="8">
         <v>1265989</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F35" s="8">
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A37" s="14">
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>2557</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B36" s="7">
         <v>2014</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C36" s="8">
         <v>3862296</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D36" s="8">
         <v>3654003</v>
       </c>
-      <c r="E37" s="11">
+      <c r="E36" s="8">
         <v>1201818</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F36" s="8">
         <v>329</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A38" s="14">
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>2558</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B37" s="7">
         <v>2015</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C37" s="8">
         <v>3800719</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D37" s="8">
         <v>3755055</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E37" s="8">
         <v>1239110</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F37" s="12">
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="12" customFormat="1" ht="17">
-      <c r="A39" s="14">
+    <row r="38" spans="1:6" s="9" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>2559</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B38" s="7">
         <v>2016</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C38" s="8">
         <v>3853151</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D38" s="8">
         <v>3814620</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E38" s="8">
         <v>1275119</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F38" s="12">
         <v>334</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>